<commit_message>
Improved metrics; new non-coro scheduler project
</commit_message>
<xml_diff>
--- a/sensor_fsm_coro/Calculations.xlsx
+++ b/sensor_fsm_coro/Calculations.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="-Os" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
   <si>
     <t>TEST_CONTROL</t>
   </si>
@@ -72,13 +73,55 @@
   </si>
   <si>
     <t>59d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2f1c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32a4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 342c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3+1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35b0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5+1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35d4</t>
+  </si>
+  <si>
+    <t>DebugLLVM</t>
+  </si>
+  <si>
+    <t>ReleaseLLVM (-Os)</t>
+  </si>
+  <si>
+    <t>average cost of coro+caller</t>
+  </si>
+  <si>
+    <t>cost of infrastructure</t>
+  </si>
+  <si>
+    <t>cost of coro overhead</t>
+  </si>
+  <si>
+    <t>cost of caller overhead</t>
+  </si>
+  <si>
+    <t>cost of coro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +155,20 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -133,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -147,6 +204,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +488,666 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>11100</v>
+      </c>
+      <c r="F4">
+        <v>140</v>
+      </c>
+      <c r="G4">
+        <v>1236</v>
+      </c>
+      <c r="H4">
+        <v>12476</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>17348</v>
+      </c>
+      <c r="F5">
+        <v>144</v>
+      </c>
+      <c r="G5">
+        <v>1256</v>
+      </c>
+      <c r="H5">
+        <v>18748</v>
+      </c>
+      <c r="I5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J10" si="0">H5-H4</f>
+        <v>6272</v>
+      </c>
+      <c r="M5">
+        <f>(2*H5)-(H4+H6)</f>
+        <v>5176</v>
+      </c>
+      <c r="O5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="6">
+        <f>J5-J6</f>
+        <v>5176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>18444</v>
+      </c>
+      <c r="F6">
+        <v>144</v>
+      </c>
+      <c r="G6">
+        <v>1256</v>
+      </c>
+      <c r="H6">
+        <v>19844</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>1096</v>
+      </c>
+      <c r="M6">
+        <f>J6-$K$8</f>
+        <v>1040</v>
+      </c>
+      <c r="O6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6">
+        <f>AVERAGE(M6:M7)</f>
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>19528</v>
+      </c>
+      <c r="F7">
+        <v>144</v>
+      </c>
+      <c r="G7">
+        <v>1256</v>
+      </c>
+      <c r="H7">
+        <v>20928</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>1084</v>
+      </c>
+      <c r="M7">
+        <f>J7-$K$8</f>
+        <v>1028</v>
+      </c>
+      <c r="O7" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7">
+        <f>P6-K8</f>
+        <v>978</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>19640</v>
+      </c>
+      <c r="F8">
+        <v>144</v>
+      </c>
+      <c r="G8">
+        <v>1256</v>
+      </c>
+      <c r="H8">
+        <v>21040</v>
+      </c>
+      <c r="I8">
+        <v>5230</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="K8">
+        <f>J8/2</f>
+        <v>56</v>
+      </c>
+      <c r="O8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P8" s="6">
+        <f>(2*P7)-J9</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>21496</v>
+      </c>
+      <c r="F9">
+        <v>144</v>
+      </c>
+      <c r="G9">
+        <v>1256</v>
+      </c>
+      <c r="H9">
+        <v>22896</v>
+      </c>
+      <c r="I9">
+        <v>5970</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>1856</v>
+      </c>
+      <c r="K9">
+        <f>J9-J7</f>
+        <v>772</v>
+      </c>
+      <c r="O9" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="6">
+        <f>(2*K8)-J10</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>21596</v>
+      </c>
+      <c r="F10">
+        <v>144</v>
+      </c>
+      <c r="G10">
+        <v>1256</v>
+      </c>
+      <c r="H10">
+        <v>22996</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>10684</v>
+      </c>
+      <c r="F15">
+        <v>140</v>
+      </c>
+      <c r="G15">
+        <v>1236</v>
+      </c>
+      <c r="H15">
+        <v>12060</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>11564</v>
+      </c>
+      <c r="F16">
+        <v>144</v>
+      </c>
+      <c r="G16">
+        <v>1256</v>
+      </c>
+      <c r="H16">
+        <v>12964</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16:J21" si="1">H16-H15</f>
+        <v>904</v>
+      </c>
+      <c r="M16">
+        <f>(2*H16)-(H15+H17)</f>
+        <v>708</v>
+      </c>
+      <c r="O16" t="s">
+        <v>26</v>
+      </c>
+      <c r="P16">
+        <f>J16-J17</f>
+        <v>708</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>11760</v>
+      </c>
+      <c r="F17">
+        <v>144</v>
+      </c>
+      <c r="G17">
+        <v>1256</v>
+      </c>
+      <c r="H17">
+        <v>13160</v>
+      </c>
+      <c r="I17">
+        <v>3368</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+      <c r="M17">
+        <f>J17-$L$6</f>
+        <v>196</v>
+      </c>
+      <c r="O17" t="s">
+        <v>25</v>
+      </c>
+      <c r="P17">
+        <f>AVERAGE(M17:M18)</f>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>11956</v>
+      </c>
+      <c r="F18">
+        <v>144</v>
+      </c>
+      <c r="G18">
+        <v>1256</v>
+      </c>
+      <c r="H18">
+        <v>13356</v>
+      </c>
+      <c r="I18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+      <c r="M18">
+        <f>J18-$L$6</f>
+        <v>196</v>
+      </c>
+      <c r="O18" t="s">
+        <v>29</v>
+      </c>
+      <c r="P18">
+        <f>P17-K19</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>12048</v>
+      </c>
+      <c r="F19">
+        <v>144</v>
+      </c>
+      <c r="G19">
+        <v>1256</v>
+      </c>
+      <c r="H19">
+        <v>13448</v>
+      </c>
+      <c r="I19">
+        <v>3488</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="K19">
+        <f>J19/2</f>
+        <v>46</v>
+      </c>
+      <c r="O19" t="s">
+        <v>27</v>
+      </c>
+      <c r="P19">
+        <f>(2*P18)-J20</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>12344</v>
+      </c>
+      <c r="F20">
+        <v>144</v>
+      </c>
+      <c r="G20">
+        <v>1256</v>
+      </c>
+      <c r="H20">
+        <v>13744</v>
+      </c>
+      <c r="I20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>296</v>
+      </c>
+      <c r="K20">
+        <f>J20-J18</f>
+        <v>100</v>
+      </c>
+      <c r="O20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P20">
+        <f>(2*K19)-J21</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>12380</v>
+      </c>
+      <c r="F21">
+        <v>144</v>
+      </c>
+      <c r="G21">
+        <v>1256</v>
+      </c>
+      <c r="H21">
+        <v>13780</v>
+      </c>
+      <c r="I21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <v>11100</v>
+        <v>10684</v>
       </c>
       <c r="F2" s="4">
         <v>140</v>
@@ -490,11 +1207,15 @@
         <v>1236</v>
       </c>
       <c r="H2" s="4">
-        <v>12476</v>
+        <v>12060</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -510,7 +1231,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4">
-        <v>17348</v>
+        <v>11564</v>
       </c>
       <c r="F3" s="4">
         <v>144</v>
@@ -519,18 +1240,20 @@
         <v>1256</v>
       </c>
       <c r="H3" s="4">
-        <v>18748</v>
+        <v>12964</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <f>H3-H2</f>
-        <v>6272</v>
-      </c>
-      <c r="M3">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" ref="J3:J8" si="0">H3-H2</f>
+        <v>904</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4">
         <f>(2*H3)-(H2+H4)</f>
-        <v>5176</v>
+        <v>708</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -547,7 +1270,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="4">
-        <v>18444</v>
+        <v>11760</v>
       </c>
       <c r="F4" s="4">
         <v>144</v>
@@ -556,22 +1279,23 @@
         <v>1256</v>
       </c>
       <c r="H4" s="4">
-        <v>19844</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4">
-        <f>H4-H3</f>
-        <v>1096</v>
-      </c>
-      <c r="K4">
+        <v>13160</v>
+      </c>
+      <c r="I4" s="4">
+        <v>3368</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="K4" s="4">
         <f>J3-J4</f>
-        <v>5176</v>
-      </c>
-      <c r="M4">
-        <f>J4-56</f>
-        <v>1040</v>
+        <v>708</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4">
+        <f>J4-$L$6</f>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -588,7 +1312,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="4">
-        <v>19528</v>
+        <v>11956</v>
       </c>
       <c r="F5" s="4">
         <v>144</v>
@@ -597,18 +1321,20 @@
         <v>1256</v>
       </c>
       <c r="H5" s="4">
-        <v>20928</v>
+        <v>13356</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5">
-        <f>H5-H4</f>
-        <v>1084</v>
-      </c>
-      <c r="M5">
-        <f>J5-56</f>
-        <v>1028</v>
+        <v>18</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4">
+        <f>J5-$L$6</f>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
@@ -625,7 +1351,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="4">
-        <v>19640</v>
+        <v>12048</v>
       </c>
       <c r="F6" s="4">
         <v>144</v>
@@ -634,15 +1360,21 @@
         <v>1256</v>
       </c>
       <c r="H6" s="4">
-        <v>21040</v>
+        <v>13448</v>
       </c>
       <c r="I6" s="4">
-        <v>5230</v>
-      </c>
-      <c r="J6">
-        <f>H6-H5</f>
-        <v>112</v>
-      </c>
+        <v>3488</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
+        <f>J6/2</f>
+        <v>46</v>
+      </c>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -652,13 +1384,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D7" s="4">
         <v>5</v>
       </c>
       <c r="E7" s="4">
-        <v>21496</v>
+        <v>12344</v>
       </c>
       <c r="F7" s="4">
         <v>144</v>
@@ -667,52 +1399,57 @@
         <v>1256</v>
       </c>
       <c r="H7" s="4">
-        <v>22896</v>
-      </c>
-      <c r="I7" s="4">
-        <v>5970</v>
-      </c>
-      <c r="J7">
-        <f>H7-H6</f>
-        <v>1856</v>
-      </c>
-      <c r="K7">
+        <v>13744</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="4">
+        <f t="shared" si="0"/>
+        <v>296</v>
+      </c>
+      <c r="K7" s="4">
         <f>J7-J5</f>
-        <v>772</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8">
-        <v>21596</v>
-      </c>
-      <c r="F8">
-        <v>144</v>
-      </c>
-      <c r="G8">
-        <v>1256</v>
-      </c>
-      <c r="H8">
-        <v>22996</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8">
-        <f>H8-H7</f>
-        <v>100</v>
-      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4">
+        <v>12380</v>
+      </c>
+      <c r="F8" s="4">
+        <v>144</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1256</v>
+      </c>
+      <c r="H8" s="4">
+        <v>13780</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -744,7 +1481,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="5">
         <v>0</v>
       </c>
       <c r="B12" s="2">
@@ -757,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <v>11100</v>
+        <v>10684</v>
       </c>
       <c r="F12" s="2">
         <v>140</v>
@@ -766,14 +1503,14 @@
         <v>1236</v>
       </c>
       <c r="H12" s="2">
-        <v>12476</v>
+        <v>12060</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="5">
         <v>1</v>
       </c>
       <c r="B13" s="2">
@@ -786,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2">
-        <v>17348</v>
+        <v>11564</v>
       </c>
       <c r="F13" s="2">
         <v>144</v>
@@ -795,14 +1532,14 @@
         <v>1256</v>
       </c>
       <c r="H13" s="2">
-        <v>18748</v>
+        <v>12964</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="5">
         <v>2</v>
       </c>
       <c r="B14" s="2">
@@ -815,7 +1552,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="2">
-        <v>18444</v>
+        <v>11760</v>
       </c>
       <c r="F14" s="2">
         <v>144</v>
@@ -824,14 +1561,14 @@
         <v>1256</v>
       </c>
       <c r="H14" s="2">
-        <v>19844</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>11</v>
+        <v>13160</v>
+      </c>
+      <c r="I14" s="2">
+        <v>3368</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="5">
         <v>3</v>
       </c>
       <c r="B15" s="2">
@@ -844,7 +1581,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="2">
-        <v>19528</v>
+        <v>11956</v>
       </c>
       <c r="F15" s="2">
         <v>144</v>
@@ -853,14 +1590,14 @@
         <v>1256</v>
       </c>
       <c r="H15" s="2">
-        <v>20928</v>
+        <v>13356</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="5">
         <v>4</v>
       </c>
       <c r="B16" s="2">
@@ -873,7 +1610,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="2">
-        <v>19640</v>
+        <v>12048</v>
       </c>
       <c r="F16" s="2">
         <v>144</v>
@@ -882,27 +1619,27 @@
         <v>1256</v>
       </c>
       <c r="H16" s="2">
-        <v>21040</v>
+        <v>13448</v>
       </c>
       <c r="I16" s="2">
-        <v>5230</v>
+        <v>3488</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="5">
         <v>5</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2">
         <v>5</v>
       </c>
       <c r="E17" s="2">
-        <v>21496</v>
+        <v>12344</v>
       </c>
       <c r="F17" s="2">
         <v>144</v>
@@ -911,27 +1648,27 @@
         <v>1256</v>
       </c>
       <c r="H17" s="2">
-        <v>22896</v>
-      </c>
-      <c r="I17" s="2">
-        <v>5970</v>
+        <v>13744</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="5">
         <v>6</v>
       </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E18" s="2">
-        <v>21596</v>
+        <v>12380</v>
       </c>
       <c r="F18" s="2">
         <v>144</v>
@@ -940,10 +1677,10 @@
         <v>1256</v>
       </c>
       <c r="H18" s="2">
-        <v>22996</v>
+        <v>13780</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>